<commit_message>
Add LaunchWin iframe handler for Customer Maintenance window searching
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A46E8-9E86-4754-8593-6AE2BFCEABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63974A0-3A82-4243-A456-C2E2EA6FBF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
   <si>
     <t>TO BE EXECUTED</t>
   </si>
@@ -587,6 +587,12 @@
   </si>
   <si>
     <t xml:space="preserve">Enter Query </t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Click New</t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="79" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1266,13 +1272,13 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K10" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
Revert to working Click logic - restore LaunchWin button clicking
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63974A0-3A82-4243-A456-C2E2EA6FBF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1895A00-69B8-4B42-9803-4984C6A770B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,9 +457,6 @@
     <t>Nationality</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -593,6 +590,9 @@
   </si>
   <si>
     <t>Click New</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="79" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1149,7 @@
         <v>27</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
@@ -1172,7 +1172,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
@@ -1192,7 +1192,7 @@
         <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K5" t="s">
         <v>37</v>
@@ -1212,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1223,7 +1223,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
@@ -1272,16 +1272,16 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1322,10 +1322,10 @@
         <v>135</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1345,10 +1345,10 @@
         <v>136</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
         <v>123</v>
       </c>
       <c r="K14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1391,10 +1391,10 @@
         <v>138</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1417,7 +1417,7 @@
         <v>127</v>
       </c>
       <c r="K16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1440,7 +1440,7 @@
         <v>127</v>
       </c>
       <c r="K17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1457,13 +1457,13 @@
         <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>129</v>
@@ -1480,13 +1480,13 @@
         <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1494,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>130</v>
@@ -1503,13 +1503,13 @@
         <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>131</v>
       </c>
       <c r="K20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1517,19 +1517,19 @@
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1537,10 +1537,10 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -1552,7 +1552,7 @@
         <v>132</v>
       </c>
       <c r="K22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1560,7 +1560,7 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>133</v>
@@ -1575,7 +1575,7 @@
         <v>75</v>
       </c>
       <c r="K23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1583,20 +1583,20 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1604,19 +1604,19 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H25" t="s">
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1633,7 +1633,7 @@
         <v>45</v>
       </c>
       <c r="I28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K28" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Add universal iframe discovery and search logic for multi-site support
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63974A0-3A82-4243-A456-C2E2EA6FBF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D0AE4-9C03-44D2-8A6B-898F3B85E9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="186">
   <si>
     <t>TO BE EXECUTED</t>
   </si>
@@ -457,9 +457,6 @@
     <t>Nationality</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
     <t>MASERU,LESOTHO</t>
   </si>
   <si>
-    <t>MALE</t>
-  </si>
-  <si>
     <t>Additional</t>
   </si>
   <si>
@@ -593,6 +587,9 @@
   </si>
   <si>
     <t>Click New</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="79" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1146,7 @@
         <v>27</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
@@ -1172,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
@@ -1192,7 +1189,7 @@
         <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
         <v>37</v>
@@ -1212,7 +1209,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1223,7 +1220,7 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
@@ -1272,16 +1269,16 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1302,7 +1299,7 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1322,10 +1319,10 @@
         <v>135</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1345,10 +1342,10 @@
         <v>136</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1371,7 +1368,7 @@
         <v>123</v>
       </c>
       <c r="K14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1391,10 +1388,10 @@
         <v>138</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1417,7 +1414,7 @@
         <v>127</v>
       </c>
       <c r="K16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1440,7 +1437,7 @@
         <v>127</v>
       </c>
       <c r="K17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1457,13 +1454,11 @@
         <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>141</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>161</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="J18" s="3"/>
       <c r="K18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>129</v>
@@ -1480,13 +1475,13 @@
         <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1494,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>130</v>
@@ -1503,13 +1498,13 @@
         <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>131</v>
       </c>
       <c r="K20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1517,19 +1512,19 @@
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1537,10 +1532,10 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -1552,7 +1547,7 @@
         <v>132</v>
       </c>
       <c r="K22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1560,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>133</v>
@@ -1575,7 +1570,7 @@
         <v>75</v>
       </c>
       <c r="K23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1583,20 +1578,20 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1604,19 +1599,19 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H25" t="s">
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1633,7 +1628,7 @@
         <v>45</v>
       </c>
       <c r="I28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K28" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Fix: Enhanced iframe detection and Ok button targeting for Account Number Generation
- Added direct ifrSubScreen iframe targeting for Ok button clicks
- Implemented CASCADE search strategy: direct ifrSubScreen -> PRIORITY 0 fallback -> general search
- Enhanced detectAndLogAllIframes() to find nested iframes using Playwright API
- Improved PRIORITY 0 logic in searchInAllSubwindows() with detailed logging
- Added detailed logging for each search phase to aid debugging
- Supports Account Number Generation dialog (ifrSubScreen) with selectors: #BTN_OK, name=BTN_OK, value=OK
- Updated documentation with all iframe detection improvements and usage examples
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450FBC8-69F1-439A-95AD-EB18376377A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DA254C-63D4-4DF8-BEBD-EB9468BBEF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t xml:space="preserve">https://10.0.46.12:7504/FCJNeoWeb/ </t>
+    <t>https://10.0.46.12:7504/FCJNeoWeb/LoginServlet</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="79" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>